<commit_message>
New archetype system implemented
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetypes/Hufflepuff.xlsx
+++ b/CoreRulebook/Data/Archetypes/Hufflepuff.xlsx
@@ -20,45 +20,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Level</t>
   </si>
   <si>
-    <t xml:space="preserve">Arcane</t>
+    <t xml:space="preserve">Expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxSpells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonuses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BasicInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token of Loyalty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Name:</t>
   </si>
   <si>
     <t xml:space="preserve">Hufflepuff Student</t>
   </si>
   <si>
-    <t xml:space="preserve">Hard{\dash}Worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student Counsellor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heart of Loyalty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ally Assist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Night-Owl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kind Heart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heart of Loyalty II</t>
+    <t xml:space="preserve">Invaluable Ally, Calming Aura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP:</t>
   </si>
   <si>
     <t xml:space="preserve">Industrious Attitude</t>
   </si>
   <si>
-    <t xml:space="preserve">Calming Aura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dedicated Training</t>
+    <t xml:space="preserve">FP:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armour:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one from: Cooking utensils, First Aid Kit, Herbology Tools. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disciplines:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose any two disciplines from the Recuperation or Divination schools. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weapons:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proficiencies:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose any two from Vitality, Conviction, Persuasion, Empathy, Observation \&amp; Nature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wand, a Student\apos{}s pack and the tools selected above. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memorised Spells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any two from the basic spells table.  </t>
   </si>
 </sst>
 </file>
@@ -73,6 +112,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,10 +130,11 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,17 +179,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -168,33 +225,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="24.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="0"/>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -203,10 +265,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="s">
+        <f aca="false">_xlfn.FLOOR.MATH((A2/4)+2)</f>
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f aca="false">IF(B2=2,"Beginner",IF(B2=3,"Novice",IF(B2=4,"Adept",IF(B2=5,"Expert",0))))</f>
+        <v>Beginner</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -214,10 +287,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
+        <f aca="false">_xlfn.FLOOR.MATH((A3/4)+2)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f aca="false">IF(B3=2,"Beginner",IF(B3=3,"Novice",IF(B3=4,"Adept",IF(B3=5,"Expert",0))))</f>
+        <v>Beginner</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,41 +309,83 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0</v>
+        <f aca="false">_xlfn.FLOOR.MATH((A4/4)+2)</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f aca="false">IF(B4=2,"Beginner",IF(B4=3,"Novice",IF(B4=4,"Adept",IF(B4=5,"Expert",0))))</f>
+        <v>Beginner</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="C5" s="5"/>
+      <c r="E5" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="5"/>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="5"/>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="5"/>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="5"/>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="5"/>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>